<commit_message>
refactor(1A): separate Itot and Imas for 'isolamento-opache' (computeItot/getImas); keep calculate() compatible
</commit_message>
<xml_diff>
--- a/pompe di calore coefficienti calcolo.xlsx
+++ b/pompe di calore coefficienti calcolo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\OneDrive\Documenti\Visual Studio Code Projects\Simulatore CT3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5324CC2-D726-4E4E-BF83-AD5004E60EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E28340-9364-4978-B4F9-ABD511A6692F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD809330-0A1B-4314-AC09-E6B59CCC375E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD809330-0A1B-4314-AC09-E6B59CCC375E}"/>
   </bookViews>
   <sheets>
     <sheet name="Pompe di calore " sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="44">
   <si>
     <t>Regolamento</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>GWP</t>
-  </si>
-  <si>
-    <t>SCOP minimo Ecodesign</t>
   </si>
   <si>
     <t>COP minimo Ecodesign</t>
@@ -141,6 +138,39 @@
       </rPr>
       <t>Efficienza stagionale minima Ecodesign [%]</t>
     </r>
+  </si>
+  <si>
+    <t>Alimentazione</t>
+  </si>
+  <si>
+    <t>Elettrica</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>aria/aria</t>
+  </si>
+  <si>
+    <t>salamoia/aria</t>
+  </si>
+  <si>
+    <t>aria/acqua – acqua/acqua</t>
+  </si>
+  <si>
+    <t>aria/acqua – acqua/acqua a acqua/acqua bassa temperatura</t>
+  </si>
+  <si>
+    <t>Salamoia/acqua</t>
+  </si>
+  <si>
+    <t>split/multisplit VRF/VRV</t>
+  </si>
+  <si>
+    <t>aria/acqua - acqua/acqua</t>
+  </si>
+  <si>
+    <t>SCOP / SPER minimo Ecodesign</t>
   </si>
 </sst>
 </file>
@@ -1056,429 +1086,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D21A575-77BF-4519-9D0E-9F70D55D896D}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I6" sqref="C6:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.36328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.1796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="20" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3">
+        <v>149</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3">
+        <v>134</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.42</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
+        <v>2.34</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3">
+        <v>137</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3">
+        <v>125</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3">
+        <v>137</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.625</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3">
+        <v>110</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3">
+        <v>110</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2.95</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3">
+        <v>125</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3">
+        <v>125</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
         <v>149</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G13" s="3">
         <v>3.8</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="F14" s="3">
+        <v>134</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.42</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3">
-        <v>134</v>
-      </c>
-      <c r="F3" s="3">
-        <v>3.42</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="3">
+        <v>137</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3.625</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="3">
+        <v>110</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="3">
+        <v>125</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
-        <v>2.34</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="3">
+        <v>130</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3">
-        <v>137</v>
-      </c>
-      <c r="F6" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3">
+        <v>130</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3">
+        <v>130</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3">
+        <v>110</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="3">
         <v>125</v>
       </c>
-      <c r="F7" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3">
-        <v>137</v>
-      </c>
-      <c r="F8" s="3">
-        <v>3.625</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3">
-        <v>110</v>
-      </c>
-      <c r="F9" s="3">
-        <v>2.8250000000000002</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3">
-        <v>110</v>
-      </c>
-      <c r="F10" s="3">
-        <v>2.95</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="G22" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="3">
         <v>125</v>
       </c>
-      <c r="F11" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3">
-        <v>125</v>
-      </c>
-      <c r="F12" s="3">
-        <v>3.3250000000000002</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="G23" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3">
-        <v>149</v>
-      </c>
-      <c r="F13" s="3">
-        <v>3.8</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="3">
-        <v>134</v>
-      </c>
-      <c r="F14" s="3">
-        <v>3.42</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="3">
-        <v>137</v>
-      </c>
-      <c r="F15" s="3">
-        <v>3.625</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="3">
-        <v>110</v>
-      </c>
-      <c r="F16" s="3">
-        <v>2.8250000000000002</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="3">
-        <v>125</v>
-      </c>
-      <c r="F17" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>